<commit_message>
Added study of dielectric relaxation when changing the bias field
</commit_message>
<xml_diff>
--- a/manuals/C_U_relaxation.xlsx
+++ b/manuals/C_U_relaxation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sfedu-my.sharepoint.com/personal/kpandryushin_sfedu_ru/Documents/programming/MegaPack v.10.10.24/Kalipso/manuals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="11_AD4DF75460589B3ACB7284850FDA45045BDEDD80" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46820C5E-3756-4060-AC22-BC8CEFF9137D}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="11_AD4DF75460589B3ACB7284850FDA45045BDEDD80" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14B6768D-C327-43DE-BF8F-2B424D36ADB9}"/>
   <bookViews>
     <workbookView xWindow="-22185" yWindow="1275" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>T</t>
-  </si>
-  <si>
     <t>V</t>
   </si>
   <si>
@@ -37,6 +34,9 @@
   </si>
   <si>
     <t>time, sec</t>
+  </si>
+  <si>
+    <t>T, K</t>
   </si>
 </sst>
 </file>
@@ -357,28 +357,28 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D17"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -389,7 +389,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -400,7 +400,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -411,7 +411,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -422,7 +422,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -433,7 +433,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -444,7 +444,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -455,10 +455,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D9">
         <v>1000</v>
@@ -466,7 +466,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -477,7 +477,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -488,7 +488,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -499,7 +499,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -510,7 +510,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -521,7 +521,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -532,7 +532,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -543,7 +543,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="C17">
         <v>2</v>

</xml_diff>

<commit_message>
added S33 and fr measuring
</commit_message>
<xml_diff>
--- a/manuals/C_U_relaxation.xlsx
+++ b/manuals/C_U_relaxation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sfedu-my.sharepoint.com/personal/kpandryushin_sfedu_ru/Documents/programming/MegaPack v.10.10.24/Kalipso/manuals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="11_AD4DF75460589B3ACB7284850FDA45045BDEDD80" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14B6768D-C327-43DE-BF8F-2B424D36ADB9}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="11_AD4DF75460589B3ACB7284850FDA45045BDEDD80" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{527F1D88-BEED-4BE2-B7DF-107D31103FB2}"/>
   <bookViews>
     <workbookView xWindow="-22185" yWindow="1275" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -357,7 +357,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -378,7 +378,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>1</v>

</xml_diff>